<commit_message>
FERRAMENTE: Desvio padrao total e com amostra
</commit_message>
<xml_diff>
--- a/media e mediana.xlsx
+++ b/media e mediana.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\code\vba-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0B3C4B5F-7ECE-4BCA-8A4B-22F7E9C606B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53C8DB77-C9C2-4B43-9918-8C56C23D7D9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1290" yWindow="1290" windowWidth="18000" windowHeight="9390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Robson</t>
   </si>
@@ -72,9 +72,6 @@
   </si>
   <si>
     <t>Nome</t>
-  </si>
-  <si>
-    <t>ANOS</t>
   </si>
   <si>
     <t>MEDIA DE IDADE</t>
@@ -90,7 +87,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +117,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -129,7 +142,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -152,55 +165,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -216,25 +185,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -298,100 +270,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>295275</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="Retângulo 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95ADDFC7-AC47-4BD1-B4AD-0C3FB6456CFA}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="2257425" y="95250"/>
-          <a:ext cx="2438400" cy="561975"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="dk1">
-            <a:shade val="50000"/>
-          </a:schemeClr>
-        </a:lnRef>
-        <a:fillRef idx="1">
-          <a:schemeClr val="dk1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="dk1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="lt1"/>
-        </a:fontRef>
-      </xdr:style>
-      <xdr:txBody>
-        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1400" baseline="0">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>MEDIA: Media de idade </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:r>
-            <a:rPr lang="pt-BR" sz="1400" baseline="0">
-              <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-              <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            </a:rPr>
-            <a:t>na tabela</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr algn="l"/>
-          <a:endParaRPr lang="pt-BR" sz="1400">
-            <a:latin typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-            <a:cs typeface="Arial" panose="020B0604020202020204" pitchFamily="34" charset="0"/>
-          </a:endParaRPr>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -671,14 +549,16 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="F1" sqref="F1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.7109375" customWidth="1"/>
-    <col min="3" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="15" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" customWidth="1"/>
+    <col min="6" max="15" width="9.140625" hidden="1" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" hidden="1"/>
   </cols>
   <sheetData>
@@ -729,10 +609,10 @@
       <c r="B6" s="3">
         <v>75</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="8"/>
+      <c r="D6" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" s="11"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -741,13 +621,11 @@
       <c r="B7" s="3">
         <v>43</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="8">
         <f>AVERAGE(Tabela1[Idade])</f>
         <v>35.636363636363633</v>
       </c>
-      <c r="E7" s="4" t="s">
-        <v>13</v>
-      </c>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
@@ -756,6 +634,8 @@
       <c r="B8" s="3">
         <v>58</v>
       </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -764,10 +644,10 @@
       <c r="B9" s="3">
         <v>41</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="10"/>
+      <c r="D9" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="12"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
@@ -776,8 +656,8 @@
       <c r="B10" s="3">
         <v>20</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>16</v>
+      <c r="D10" s="16" t="s">
+        <v>15</v>
       </c>
       <c r="E10" s="13"/>
     </row>
@@ -788,13 +668,11 @@
       <c r="B11" s="3">
         <v>22</v>
       </c>
-      <c r="D11" s="11">
+      <c r="D11" s="4">
         <f>MEDIAN(B2:B12)</f>
         <v>32</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>13</v>
-      </c>
+      <c r="E11" s="14"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
@@ -805,8 +683,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="5"/>
@@ -815,16 +692,16 @@
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="6"/>
       <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="D16" s="9"/>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="6"/>
       <c r="C17" s="5"/>
@@ -832,21 +709,21 @@
       <c r="F17" s="5"/>
       <c r="G17" s="5"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6"/>
       <c r="C18" s="5"/>
       <c r="D18" s="5"/>
       <c r="G18" s="5"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="G19" s="5"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
       <c r="B20" s="6"/>
       <c r="C20" s="5"/>
@@ -854,7 +731,7 @@
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="5"/>
       <c r="B21" s="6"/>
       <c r="C21" s="5"/>
@@ -863,7 +740,7 @@
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="5"/>
       <c r="B22" s="6"/>
       <c r="C22" s="5"/>
@@ -872,7 +749,7 @@
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="5"/>
       <c r="B23" s="6"/>
       <c r="C23" s="5"/>
@@ -881,7 +758,7 @@
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="5"/>
       <c r="B24" s="6"/>
       <c r="C24" s="5"/>
@@ -890,7 +767,7 @@
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
       <c r="B25" s="6"/>
       <c r="C25" s="5"/>
@@ -899,7 +776,7 @@
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5"/>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -918,16 +795,10 @@
     <row r="40" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
     <row r="41" customFormat="1" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E10"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <drawing r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>